<commit_message>
update file feedback KH
</commit_message>
<xml_diff>
--- a/Bug_Report/Bug Khemarama..xlsx
+++ b/Bug_Report/Bug Khemarama..xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\vpba\Bug_Report\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Bỏ chữ không có kết quả phù hợp với từ khoá tìm kiếm.</t>
   </si>
@@ -48,12 +43,6 @@
   </si>
   <si>
     <t>Mô tả bug</t>
-  </si>
-  <si>
-    <t>How to fix</t>
-  </si>
-  <si>
-    <t>Refer</t>
   </si>
   <si>
     <t>Lỗi link banner ở sidebar không hoạt động.
@@ -72,9 +61,6 @@
     <t>Category - khi không có bài viết</t>
   </si>
   <si>
-    <t>Path file</t>
-  </si>
-  <si>
     <t xml:space="preserve">Category  </t>
   </si>
   <si>
@@ -84,8 +70,50 @@
     <t>Trang chủ</t>
   </si>
   <si>
+    <t>move get_footer(); to out "container" class.</t>
+  </si>
+  <si>
+    <t>\wp-content\themes\vpba\index.php</t>
+  </si>
+  <si>
+    <t>\wp-content\themes\vpba\single-story.php</t>
+  </si>
+  <si>
+    <t>Update format html</t>
+  </si>
+  <si>
+    <t>Image1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add URL to image </t>
+  </si>
+  <si>
+    <t>\wp-content\themes\vpba\action\sidebar\render\slider.php</t>
+  </si>
+  <si>
+    <t>Click vào dấu + và search tool Custom HTML</t>
+  </si>
+  <si>
+    <t>Vào video youtube cần embed lên web, nhấn chuột phải chọn "Sao chép mã nhúng"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paste mã vừa sao chép sang block chọn hiển thị video </t>
+  </si>
+  <si>
+    <t>Dán xong thì nhấn preview để check xem thử.</t>
+  </si>
+  <si>
+    <t>Điều chỉnh width và height theo độ dài và độ rộng muốn hiện thị lên trang web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoặc thêm dòng  style="max-width:100%"  để hiển thị full kích thước cho phép trên web </t>
+  </si>
+  <si>
+    <t>embed_youtube</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Delete "else" handle as follows:
+      <t xml:space="preserve">Xóa code bên dưới
 &lt;?php	
 	endwhile;
 </t>
@@ -120,10 +148,11 @@
       </rPr>
       <t>endif;</t>
     </r>
+    <phoneticPr fontId="7"/>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">delete "span" tag as follows:
+      <t xml:space="preserve">Xóa code bên dưới
 </t>
     </r>
     <r>
@@ -136,58 +165,105 @@
       </rPr>
       <t>&lt;span class="article_category_info"&gt;Tác giả: &lt;span&gt;&lt;?php echo get_the_author(); ?&gt;&lt;/span&gt;&lt;/span&gt;&lt;br&gt;</t>
     </r>
-  </si>
-  <si>
-    <t>move get_footer(); to out "container" class.</t>
-  </si>
-  <si>
-    <t>\wp-content\themes\vpba\index.php</t>
-  </si>
-  <si>
-    <t>\wp-content\themes\vpba\single-story.php</t>
-  </si>
-  <si>
-    <t>Update format html</t>
-  </si>
-  <si>
-    <t>Image1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add URL to image </t>
-  </si>
-  <si>
-    <t>\wp-content\themes\vpba\action\sidebar\render\slider.php</t>
-  </si>
-  <si>
-    <t>embed youtube link in the post is currently having some problems so please refer to how to embed it on the ref page.</t>
-  </si>
-  <si>
-    <t>Click vào dấu + và search tool Custom HTML</t>
-  </si>
-  <si>
-    <t>Vào video youtube cần embed lên web, nhấn chuột phải chọn "Sao chép mã nhúng"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paste mã vừa sao chép sang block chọn hiển thị video </t>
-  </si>
-  <si>
-    <t>Dán xong thì nhấn preview để check xem thử.</t>
-  </si>
-  <si>
-    <t>Điều chỉnh width và height theo độ dài và độ rộng muốn hiện thị lên trang web</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hoặc thêm dòng  style="max-width:100%"  để hiển thị full kích thước cho phép trên web </t>
-  </si>
-  <si>
-    <t>embed_youtube</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>em lại css menu footer
+giúp tìm nguyên nhân bị mất css footer (http://khemarama.net/)</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">xoá sidebar nằm bên trong </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>detail post và detail story</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>tìm kiếm đưa xuống sidebar</t>
+  </si>
+  <si>
+    <t>thêm field des cho post và trang chủ sẽ get từ field des</t>
+  </si>
+  <si>
+    <r>
+      <t>Cá</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ch fix</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <t>Nơ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i sửa</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ham khảo</t>
+    </r>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>- Body fontsize 15
+- Tiêu đề font 26
+- Tiêu đề detail post và story thì luôn luôn canh ở  giữa Và Capitalize Each Word. 
+- Nội dung bài post và story canh đều 2 bên
+- Tiêu đề màu chữ RGB(192, 0, 0)
+- Màu chữ toàn trang RGB(0, 32,  96)</t>
+    <phoneticPr fontId="7"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -228,6 +304,18 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -329,7 +417,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -387,6 +475,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -429,12 +519,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1185,7 +1282,7 @@
         <xdr:cNvPr id="2" name="image1.png" title="Hình ảnh">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE90EB6A-C0AA-4661-B418-F0AAAAE12883}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FE90EB6A-C0AA-4661-B418-F0AAAAE12883}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1417,21 +1514,21 @@
   <dimension ref="B2:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
     <col min="5" max="5" width="62" customWidth="1"/>
     <col min="6" max="6" width="45" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1439,39 +1536,39 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="102" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="105.6" x14ac:dyDescent="0.25">
       <c r="B4" s="8">
         <v>2</v>
       </c>
@@ -1479,10 +1576,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>3</v>
@@ -1490,51 +1587,49 @@
       <c r="G4" s="19"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="2:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="24">
+    <row r="5" spans="2:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="26">
         <v>3</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>21</v>
+      <c r="D5" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="20"/>
     </row>
-    <row r="6" spans="2:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="25"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="29"/>
+    <row r="6" spans="2:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="27"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G6" s="20"/>
     </row>
-    <row r="7" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8">
         <v>4</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="14"/>
-      <c r="E7" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="E7" s="11"/>
       <c r="F7" s="12"/>
       <c r="G7" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>5</v>
       </c>
@@ -1546,87 +1641,107 @@
       <c r="F8" s="16"/>
       <c r="G8" s="20"/>
     </row>
-    <row r="9" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="31">
+    <row r="9" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="33">
         <v>6</v>
       </c>
-      <c r="C9" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>22</v>
+      <c r="C9" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>17</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="19"/>
     </row>
-    <row r="10" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="32"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="30"/>
+    <row r="10" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="34"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="21"/>
+    <row r="11" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G11" s="19"/>
     </row>
-    <row r="12" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+    <row r="12" spans="2:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>7</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>33</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="4"/>
       <c r="F12" s="6"/>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
+    <row r="13" spans="2:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="8">
+        <v>8</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="D13" s="10"/>
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
       <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+    <row r="14" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
+    <row r="15" spans="2:9" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="8">
+        <v>10</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="D15" s="10"/>
       <c r="E15" s="11"/>
       <c r="F15" s="12"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+    <row r="16" spans="2:9" ht="109.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>11</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>40</v>
+      </c>
       <c r="D16" s="5"/>
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
@@ -1634,7 +1749,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
@@ -1642,7 +1757,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
@@ -1650,7 +1765,7 @@
       <c r="F19" s="12"/>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
@@ -1658,7 +1773,7 @@
       <c r="F20" s="6"/>
       <c r="G20" s="20"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
@@ -1666,7 +1781,7 @@
       <c r="F21" s="12"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
@@ -1674,7 +1789,7 @@
       <c r="F22" s="6"/>
       <c r="G22" s="20"/>
     </row>
-    <row r="23" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
@@ -1682,7 +1797,7 @@
       <c r="F23" s="12"/>
       <c r="G23" s="19"/>
     </row>
-    <row r="24" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="5"/>
@@ -1690,7 +1805,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="20"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
@@ -1698,7 +1813,7 @@
       <c r="F25" s="12"/>
       <c r="G25" s="19"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="5"/>
@@ -1717,6 +1832,7 @@
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
   </mergeCells>
+  <phoneticPr fontId="7"/>
   <hyperlinks>
     <hyperlink ref="G3" location="image_confirm!B2" display="Image1"/>
   </hyperlinks>
@@ -1729,79 +1845,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E3:U161"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="6:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="F3" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-    </row>
-    <row r="41" spans="5:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="E41" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-    </row>
-    <row r="83" spans="6:21" ht="15" x14ac:dyDescent="0.2">
-      <c r="F83" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="G83" s="35"/>
-      <c r="H83" s="35"/>
-      <c r="I83" s="35"/>
-      <c r="J83" s="35"/>
-      <c r="K83" s="35"/>
-      <c r="L83" s="35"/>
-      <c r="Q83" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="R83" s="35"/>
-      <c r="S83" s="35"/>
-      <c r="T83" s="35"/>
-      <c r="U83" s="35"/>
-    </row>
-    <row r="121" spans="7:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="G121" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="H121" s="35"/>
-      <c r="I121" s="35"/>
-      <c r="J121" s="35"/>
-      <c r="K121" s="35"/>
-      <c r="L121" s="35"/>
-      <c r="M121" s="35"/>
-      <c r="N121" s="35"/>
-      <c r="O121" s="35"/>
-    </row>
-    <row r="161" spans="7:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="G161" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="H161" s="35"/>
-      <c r="I161" s="35"/>
-      <c r="J161" s="35"/>
-      <c r="K161" s="35"/>
-      <c r="L161" s="35"/>
-      <c r="M161" s="35"/>
-      <c r="N161" s="35"/>
-      <c r="O161" s="35"/>
-      <c r="P161" s="35"/>
+    <row r="3" spans="6:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="F3" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="41" spans="5:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="E41" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+      <c r="L41" s="22"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+    </row>
+    <row r="83" spans="6:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="F83" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G83" s="21"/>
+      <c r="H83" s="21"/>
+      <c r="I83" s="21"/>
+      <c r="J83" s="21"/>
+      <c r="K83" s="21"/>
+      <c r="L83" s="21"/>
+      <c r="Q83" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="R83" s="21"/>
+      <c r="S83" s="21"/>
+      <c r="T83" s="21"/>
+      <c r="U83" s="21"/>
+    </row>
+    <row r="121" spans="7:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="G121" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H121" s="21"/>
+      <c r="I121" s="21"/>
+      <c r="J121" s="21"/>
+      <c r="K121" s="21"/>
+      <c r="L121" s="21"/>
+      <c r="M121" s="21"/>
+      <c r="N121" s="21"/>
+      <c r="O121" s="21"/>
+    </row>
+    <row r="161" spans="7:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="G161" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H161" s="21"/>
+      <c r="I161" s="21"/>
+      <c r="J161" s="21"/>
+      <c r="K161" s="21"/>
+      <c r="L161" s="21"/>
+      <c r="M161" s="21"/>
+      <c r="N161" s="21"/>
+      <c r="O161" s="21"/>
+      <c r="P161" s="21"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1816,17 +1933,18 @@
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
move form search xuống sidebar
</commit_message>
<xml_diff>
--- a/Bug_Report/Bug Khemarama..xlsx
+++ b/Bug_Report/Bug Khemarama..xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\vpba\Bug_Report\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Bỏ chữ không có kết quả phù hợp với từ khoá tìm kiếm.</t>
   </si>
@@ -258,12 +263,24 @@
 - Màu chữ toàn trang RGB(0, 32,  96)</t>
     <phoneticPr fontId="7"/>
   </si>
+  <si>
+    <t>Nội dung rút gọn sẽ được get từ excerpt thay vì lấy phần đầu của content</t>
+  </si>
+  <si>
+    <t>\wp-content\themes\vpba\action\category\render\template-category</t>
+  </si>
+  <si>
+    <t>Đã move xuống sidebar</t>
+  </si>
+  <si>
+    <t>\wp-content\themes\vpba\template-parts\search\index.php</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -417,7 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -480,6 +497,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -519,19 +548,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1282,7 +1308,7 @@
         <xdr:cNvPr id="2" name="image1.png" title="Hình ảnh">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FE90EB6A-C0AA-4661-B418-F0AAAAE12883}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE90EB6A-C0AA-4661-B418-F0AAAAE12883}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1513,22 +1539,22 @@
   </sheetPr>
   <dimension ref="B2:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="41.109375" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
     <col min="5" max="5" width="62" customWidth="1"/>
     <col min="6" max="6" width="45" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" ht="15.75" customHeight="1">
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1538,17 +1564,17 @@
       <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="38.25">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -1568,7 +1594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="102">
       <c r="B4" s="8">
         <v>2</v>
       </c>
@@ -1587,17 +1613,17 @@
       <c r="G4" s="19"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="2:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="26">
+    <row r="5" spans="2:9" ht="39.75" customHeight="1">
+      <c r="B5" s="30">
         <v>3</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="34" t="s">
         <v>32</v>
       </c>
       <c r="F5" s="13" t="s">
@@ -1605,17 +1631,17 @@
       </c>
       <c r="G5" s="20"/>
     </row>
-    <row r="6" spans="2:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="27"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="31"/>
+    <row r="6" spans="2:9" ht="39.75" customHeight="1">
+      <c r="B6" s="31"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="35"/>
       <c r="F6" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G6" s="20"/>
     </row>
-    <row r="7" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="29.25" customHeight="1">
       <c r="B7" s="8">
         <v>4</v>
       </c>
@@ -1629,7 +1655,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="15.75" customHeight="1">
       <c r="B8" s="4">
         <v>5</v>
       </c>
@@ -1641,17 +1667,17 @@
       <c r="F8" s="16"/>
       <c r="G8" s="20"/>
     </row>
-    <row r="9" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="33">
+    <row r="9" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B9" s="37">
         <v>6</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="36" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="17" t="s">
@@ -1659,20 +1685,20 @@
       </c>
       <c r="G9" s="19"/>
     </row>
-    <row r="10" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="34"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="32"/>
+    <row r="10" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B10" s="38"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="36"/>
       <c r="F10" s="11" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="23"/>
+    <row r="11" spans="2:9" ht="15.75" customHeight="1">
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="11" t="s">
         <v>20</v>
       </c>
@@ -1681,11 +1707,11 @@
       </c>
       <c r="G11" s="19"/>
     </row>
-    <row r="12" spans="2:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="50.45" customHeight="1">
       <c r="B12" s="4">
         <v>7</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="24" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="5"/>
@@ -1693,7 +1719,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="2:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="50.45" customHeight="1">
       <c r="B13" s="8">
         <v>8</v>
       </c>
@@ -1705,35 +1731,47 @@
       <c r="F13" s="12"/>
       <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="26.25" customHeight="1">
       <c r="B14" s="4">
         <v>9</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="6"/>
+      <c r="D14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>44</v>
+      </c>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="2:9" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" ht="25.9" customHeight="1">
       <c r="B15" s="8">
         <v>10</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
+      <c r="D15" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>42</v>
+      </c>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="2:9" ht="109.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" ht="109.15" customHeight="1">
       <c r="B16" s="4">
         <v>11</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="26" t="s">
         <v>40</v>
       </c>
       <c r="D16" s="5"/>
@@ -1741,7 +1779,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1">
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
@@ -1749,7 +1787,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="15.75" customHeight="1">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
@@ -1757,7 +1795,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="15.75" customHeight="1">
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
@@ -1765,7 +1803,7 @@
       <c r="F19" s="12"/>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="15.75" customHeight="1">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
@@ -1773,7 +1811,7 @@
       <c r="F20" s="6"/>
       <c r="G20" s="20"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="15.75" customHeight="1">
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
@@ -1781,7 +1819,7 @@
       <c r="F21" s="12"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="12.75">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="5"/>
@@ -1789,7 +1827,7 @@
       <c r="F22" s="6"/>
       <c r="G22" s="20"/>
     </row>
-    <row r="23" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="12.75">
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
@@ -1797,7 +1835,7 @@
       <c r="F23" s="12"/>
       <c r="G23" s="19"/>
     </row>
-    <row r="24" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="12.75">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="5"/>
@@ -1805,7 +1843,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="20"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1">
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
@@ -1813,7 +1851,7 @@
       <c r="F25" s="12"/>
       <c r="G25" s="19"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="5"/>
@@ -1847,9 +1885,9 @@
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="3" spans="6:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="6:10" ht="15">
       <c r="F3" s="22" t="s">
         <v>24</v>
       </c>
@@ -1858,7 +1896,7 @@
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
     </row>
-    <row r="41" spans="5:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:14" ht="15">
       <c r="E41" s="22" t="s">
         <v>25</v>
       </c>
@@ -1872,7 +1910,7 @@
       <c r="M41" s="21"/>
       <c r="N41" s="21"/>
     </row>
-    <row r="83" spans="6:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="6:21" ht="15">
       <c r="F83" s="22" t="s">
         <v>26</v>
       </c>
@@ -1890,7 +1928,7 @@
       <c r="T83" s="21"/>
       <c r="U83" s="21"/>
     </row>
-    <row r="121" spans="7:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="121" spans="7:15" ht="15">
       <c r="G121" s="22" t="s">
         <v>28</v>
       </c>
@@ -1903,7 +1941,7 @@
       <c r="N121" s="21"/>
       <c r="O121" s="21"/>
     </row>
-    <row r="161" spans="7:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="161" spans="7:16" ht="15">
       <c r="G161" s="22" t="s">
         <v>29</v>
       </c>
@@ -1933,12 +1971,12 @@
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" s="2" t="s">
         <v>21</v>
       </c>

</xml_diff>